<commit_message>
Updated Test data for login
</commit_message>
<xml_diff>
--- a/TestData/OpenCart_LoginData.xlsx
+++ b/TestData/OpenCart_LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harshit bisht\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC144A92-D9C6-4315-AD5F-5072612D49A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208ECCE4-234F-4FCC-88C6-C0C9ACDC2EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -470,7 +470,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +510,7 @@
         <v>123</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>